<commit_message>
Update: -Everything for the CS6375 homework 2 program was updated. Fixed Logistic Regression. Hooray!
</commit_message>
<xml_diff>
--- a/projects/graduate/cs6375/homework2/results.xlsx
+++ b/projects/graduate/cs6375/homework2/results.xlsx
@@ -45,7 +45,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J11" authorId="0">
+    <comment ref="J10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="15">
   <si>
     <t>Discard Length</t>
   </si>
@@ -177,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -206,6 +206,7 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+      <selection activeCell="L16" sqref="L16:L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -735,43 +736,73 @@
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" spans="1:10" s="1" customFormat="1">
-      <c r="A11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="A11" s="1">
         <v>1</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>0</v>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1">
+        <v>3</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
+      </c>
+      <c r="E11" s="1">
+        <v>50</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="G11" s="6">
+        <v>-0.1</v>
+      </c>
+      <c r="H11">
+        <v>11.4817</v>
+      </c>
+      <c r="I11" s="10">
+        <v>0.92050200000000004</v>
+      </c>
+      <c r="J11">
+        <f>I11/H11</f>
+        <v>8.017122899919002E-2</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
@@ -786,25 +817,25 @@
         <v>50</v>
       </c>
       <c r="F12" s="6">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="G12" s="6">
         <v>-0.1</v>
       </c>
       <c r="H12">
-        <v>8.8171300000000006</v>
+        <v>11.524699999999999</v>
       </c>
       <c r="I12" s="10">
-        <v>0.72803300000000004</v>
+        <v>0.93305400000000005</v>
       </c>
       <c r="J12">
-        <f>I12/H12</f>
-        <v>8.2570292147217977E-2</v>
+        <f t="shared" ref="J12:J28" si="1">I12/H12</f>
+        <v>8.0961239771968049E-2</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
@@ -819,25 +850,25 @@
         <v>50</v>
       </c>
       <c r="F13" s="6">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G13" s="6">
         <v>-0.1</v>
       </c>
       <c r="H13">
-        <v>9.0358999999999998</v>
-      </c>
-      <c r="I13" s="10">
-        <v>0.72803300000000004</v>
+        <v>10.808299999999999</v>
+      </c>
+      <c r="I13" s="12">
+        <v>0.94351499999999999</v>
       </c>
       <c r="J13">
-        <f t="shared" ref="J13:J23" si="1">I13/H13</f>
-        <v>8.0571166126229818E-2</v>
+        <f t="shared" si="1"/>
+        <v>8.7295411859404357E-2</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
@@ -849,28 +880,28 @@
         <v>6</v>
       </c>
       <c r="E14" s="1">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F14" s="6">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="G14" s="6">
         <v>-0.1</v>
       </c>
       <c r="H14">
-        <v>8.5579300000000007</v>
-      </c>
-      <c r="I14" s="11">
-        <v>0.73012600000000005</v>
+        <v>21.738900000000001</v>
+      </c>
+      <c r="I14" s="10">
+        <v>0.92677799999999999</v>
       </c>
       <c r="J14">
-        <f t="shared" si="1"/>
-        <v>8.5315724713803456E-2</v>
+        <f>I14/H14</f>
+        <v>4.2632239901742953E-2</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B15" t="s">
         <v>9</v>
@@ -879,31 +910,31 @@
         <v>3</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E15" s="1">
         <v>100</v>
       </c>
       <c r="F15" s="6">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="G15" s="6">
         <v>-0.1</v>
       </c>
       <c r="H15">
-        <v>13.093299999999999</v>
-      </c>
-      <c r="I15" s="10">
-        <v>0.72803300000000004</v>
+        <v>19.9237</v>
+      </c>
+      <c r="I15" s="11">
+        <v>0.94769899999999996</v>
       </c>
       <c r="J15">
-        <f t="shared" si="1"/>
-        <v>5.5603476587262196E-2</v>
+        <f t="shared" ref="J15:J16" si="2">I15/H15</f>
+        <v>4.756641587656911E-2</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
         <v>9</v>
@@ -912,31 +943,31 @@
         <v>3</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E16" s="1">
         <v>100</v>
       </c>
       <c r="F16" s="6">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G16" s="6">
         <v>-0.1</v>
       </c>
       <c r="H16">
-        <v>12.940899999999999</v>
-      </c>
-      <c r="I16" s="10">
-        <v>0.72803300000000004</v>
+        <v>18.0458</v>
+      </c>
+      <c r="I16" s="12">
+        <v>0.94560699999999998</v>
       </c>
       <c r="J16">
-        <f t="shared" si="1"/>
-        <v>5.6258297336352195E-2</v>
+        <f t="shared" si="2"/>
+        <v>5.2400392335058575E-2</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s">
         <v>9</v>
@@ -948,130 +979,130 @@
         <v>7</v>
       </c>
       <c r="E17" s="1">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F17" s="6">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="G17" s="6">
         <v>-0.1</v>
       </c>
       <c r="H17">
-        <v>13.8842</v>
+        <v>9.9088799999999999</v>
       </c>
       <c r="I17" s="10">
-        <v>0.72803300000000004</v>
+        <v>0.93096199999999996</v>
       </c>
       <c r="J17">
         <f t="shared" si="1"/>
-        <v>5.2436078420074618E-2</v>
+        <v>9.3952293296517872E-2</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C18" s="1">
         <v>3</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E18" s="1">
         <v>50</v>
       </c>
       <c r="F18" s="6">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="G18" s="6">
         <v>-0.1</v>
       </c>
       <c r="H18">
-        <v>8.3722999999999992</v>
-      </c>
-      <c r="I18" s="10">
-        <v>0.72803300000000004</v>
+        <v>9.85426</v>
+      </c>
+      <c r="I18" s="12">
+        <v>0.92886999999999997</v>
       </c>
       <c r="J18">
         <f t="shared" si="1"/>
-        <v>8.6957347443354885E-2</v>
+        <v>9.4260756261758866E-2</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C19" s="1">
         <v>3</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E19" s="1">
         <v>50</v>
       </c>
       <c r="F19" s="6">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G19" s="6">
         <v>-0.1</v>
       </c>
-      <c r="H19">
-        <v>8.3407800000000005</v>
+      <c r="H19" s="8">
+        <v>9.23963</v>
       </c>
       <c r="I19" s="10">
-        <v>0.72803300000000004</v>
-      </c>
-      <c r="J19">
+        <v>0.92468600000000001</v>
+      </c>
+      <c r="J19" s="8">
         <f t="shared" si="1"/>
-        <v>8.728596126501359E-2</v>
+        <v>0.10007824988662967</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="1">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
         <v>9</v>
       </c>
-      <c r="B20" t="s">
-        <v>8</v>
-      </c>
       <c r="C20" s="1">
         <v>3</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E20" s="1">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F20" s="6">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="G20" s="6">
         <v>-0.1</v>
       </c>
-      <c r="H20" s="8">
-        <v>8.2970100000000002</v>
+      <c r="H20">
+        <v>19.9602</v>
       </c>
       <c r="I20" s="10">
-        <v>0.72803300000000004</v>
-      </c>
-      <c r="J20" s="8">
-        <f t="shared" si="1"/>
-        <v>8.774642913531501E-2</v>
+        <v>0.93096199999999996</v>
+      </c>
+      <c r="J20">
+        <f t="shared" ref="J20:J22" si="3">I20/H20</f>
+        <v>4.6640915421689161E-2</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C21" s="1">
         <v>3</v>
@@ -1083,28 +1114,28 @@
         <v>100</v>
       </c>
       <c r="F21" s="6">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="G21" s="6">
         <v>-0.1</v>
       </c>
       <c r="H21">
-        <v>13.3583</v>
-      </c>
-      <c r="I21" s="10">
-        <v>0.72803300000000004</v>
+        <v>19.586300000000001</v>
+      </c>
+      <c r="I21" s="12">
+        <v>0.92468600000000001</v>
       </c>
       <c r="J21">
-        <f t="shared" si="1"/>
-        <v>5.4500422958011129E-2</v>
+        <f t="shared" si="3"/>
+        <v>4.721085656811138E-2</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B22" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C22" s="1">
         <v>3</v>
@@ -1116,25 +1147,25 @@
         <v>100</v>
       </c>
       <c r="F22" s="6">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G22" s="6">
         <v>-0.1</v>
       </c>
       <c r="H22">
-        <v>12.947699999999999</v>
+        <v>18.817399999999999</v>
       </c>
       <c r="I22" s="10">
-        <v>0.72803300000000004</v>
+        <v>0.93096199999999996</v>
       </c>
       <c r="J22">
-        <f t="shared" si="1"/>
-        <v>5.6228751052310455E-2</v>
+        <f t="shared" si="3"/>
+        <v>4.9473466047381676E-2</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B23" t="s">
         <v>8</v>
@@ -1143,78 +1174,417 @@
         <v>3</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E23" s="1">
+        <v>50</v>
+      </c>
+      <c r="F23" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="G23" s="6">
+        <v>-0.1</v>
+      </c>
+      <c r="H23">
+        <v>11.605499999999999</v>
+      </c>
+      <c r="I23" s="10">
+        <v>0.94142300000000001</v>
+      </c>
+      <c r="J23">
+        <f>I23/H23</f>
+        <v>8.111869372280385E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="1">
+        <v>14</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="1">
+        <v>3</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="1">
+        <v>50</v>
+      </c>
+      <c r="F24" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="G24" s="6">
+        <v>-0.1</v>
+      </c>
+      <c r="H24">
+        <v>11.4962</v>
+      </c>
+      <c r="I24" s="10">
+        <v>0.94351499999999999</v>
+      </c>
+      <c r="J24">
+        <f t="shared" ref="J24:J34" si="4">I24/H24</f>
+        <v>8.2071902019797846E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="1">
+        <v>15</v>
+      </c>
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="1">
+        <v>3</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="1">
+        <v>50</v>
+      </c>
+      <c r="F25" s="6">
+        <v>1</v>
+      </c>
+      <c r="G25" s="6">
+        <v>-0.1</v>
+      </c>
+      <c r="H25">
+        <v>11.246</v>
+      </c>
+      <c r="I25" s="12">
+        <v>0.94351499999999999</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="4"/>
+        <v>8.3897830339676321E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="1">
+        <v>16</v>
+      </c>
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="1">
+        <v>3</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="1">
         <v>100</v>
       </c>
-      <c r="F23" s="6">
+      <c r="F26" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="G26" s="6">
+        <v>-0.1</v>
+      </c>
+      <c r="H26">
+        <v>21.107800000000001</v>
+      </c>
+      <c r="I26" s="10">
+        <v>0.94351499999999999</v>
+      </c>
+      <c r="J26">
+        <f>I26/H26</f>
+        <v>4.4699826604383208E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="1">
+        <v>17</v>
+      </c>
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="1">
+        <v>3</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="1">
+        <v>100</v>
+      </c>
+      <c r="F27" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="G27" s="6">
+        <v>-0.1</v>
+      </c>
+      <c r="H27">
+        <v>20.374700000000001</v>
+      </c>
+      <c r="I27" s="11">
+        <v>0.94769899999999996</v>
+      </c>
+      <c r="J27">
+        <f t="shared" ref="J27:J34" si="5">I27/H27</f>
+        <v>4.6513519217460865E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="1">
+        <v>18</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="1">
+        <v>3</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="1">
+        <v>100</v>
+      </c>
+      <c r="F28" s="6">
         <v>1</v>
       </c>
-      <c r="G23" s="6">
-        <v>-0.1</v>
-      </c>
-      <c r="H23">
-        <v>13.260300000000001</v>
-      </c>
-      <c r="I23" s="10">
-        <v>0.72803300000000004</v>
-      </c>
-      <c r="J23">
-        <f t="shared" si="1"/>
-        <v>5.4903207318084811E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="F24" s="5"/>
-      <c r="I24" s="10"/>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="F25" s="5"/>
-      <c r="I25" s="10"/>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="F26" s="5"/>
-      <c r="I26" s="10"/>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="F27" s="5"/>
-      <c r="I27" s="10"/>
-    </row>
-    <row r="28" spans="1:10">
-      <c r="F28" s="5"/>
-      <c r="I28" s="10"/>
+      <c r="G28" s="6">
+        <v>-0.1</v>
+      </c>
+      <c r="H28">
+        <v>18.721299999999999</v>
+      </c>
+      <c r="I28" s="12">
+        <v>0.94560699999999998</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="5"/>
+        <v>5.0509686827303661E-2</v>
+      </c>
     </row>
     <row r="29" spans="1:10">
-      <c r="F29" s="5"/>
-      <c r="I29" s="10"/>
+      <c r="A29" s="1">
+        <v>19</v>
+      </c>
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="1">
+        <v>3</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="1">
+        <v>50</v>
+      </c>
+      <c r="F29" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="G29" s="6">
+        <v>-0.1</v>
+      </c>
+      <c r="H29">
+        <v>10.183</v>
+      </c>
+      <c r="I29" s="10">
+        <v>0.93096199999999996</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="5"/>
+        <v>9.1423156240793474E-2</v>
+      </c>
     </row>
     <row r="30" spans="1:10">
-      <c r="F30" s="5"/>
-      <c r="I30" s="10"/>
+      <c r="A30" s="1">
+        <v>20</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="1">
+        <v>3</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="1">
+        <v>50</v>
+      </c>
+      <c r="F30" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="G30" s="6">
+        <v>-0.1</v>
+      </c>
+      <c r="H30">
+        <v>9.8260799999999993</v>
+      </c>
+      <c r="I30" s="12">
+        <v>0.92886999999999997</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="5"/>
+        <v>9.4531084623776726E-2</v>
+      </c>
     </row>
     <row r="31" spans="1:10">
-      <c r="F31" s="5"/>
-      <c r="I31" s="10"/>
+      <c r="A31" s="1">
+        <v>21</v>
+      </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="1">
+        <v>3</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="1">
+        <v>50</v>
+      </c>
+      <c r="F31" s="6">
+        <v>1</v>
+      </c>
+      <c r="G31" s="6">
+        <v>-0.1</v>
+      </c>
+      <c r="H31">
+        <v>9.4154800000000005</v>
+      </c>
+      <c r="I31" s="10">
+        <v>0.92468600000000001</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="5"/>
+        <v>9.8209119450097068E-2</v>
+      </c>
     </row>
     <row r="32" spans="1:10">
-      <c r="F32" s="4"/>
-      <c r="I32" s="10"/>
-    </row>
-    <row r="33" spans="6:6">
-      <c r="F33" s="4"/>
-    </row>
-    <row r="34" spans="6:6">
-      <c r="F34" s="4"/>
-    </row>
-    <row r="35" spans="6:6">
-      <c r="F35" s="4"/>
-    </row>
-    <row r="36" spans="6:6">
-      <c r="F36" s="4"/>
-    </row>
-    <row r="37" spans="6:6">
-      <c r="F37" s="4"/>
+      <c r="A32" s="1">
+        <v>22</v>
+      </c>
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="1">
+        <v>3</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="1">
+        <v>100</v>
+      </c>
+      <c r="F32" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="G32" s="6">
+        <v>-0.1</v>
+      </c>
+      <c r="H32">
+        <v>20.172799999999999</v>
+      </c>
+      <c r="I32" s="10">
+        <v>0.93096199999999996</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="5"/>
+        <v>4.6149369447969546E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="1">
+        <v>23</v>
+      </c>
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="1">
+        <v>3</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="1">
+        <v>100</v>
+      </c>
+      <c r="F33" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="G33" s="6">
+        <v>-0.1</v>
+      </c>
+      <c r="H33">
+        <v>18.973400000000002</v>
+      </c>
+      <c r="I33" s="12">
+        <v>0.92468600000000001</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="5"/>
+        <v>4.8735914490813451E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="1">
+        <v>24</v>
+      </c>
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="1">
+        <v>3</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="1">
+        <v>100</v>
+      </c>
+      <c r="F34" s="6">
+        <v>1</v>
+      </c>
+      <c r="G34" s="6">
+        <v>-0.1</v>
+      </c>
+      <c r="H34" s="8">
+        <v>16.800699999999999</v>
+      </c>
+      <c r="I34" s="10">
+        <v>0.93096199999999996</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="5"/>
+        <v>5.5412095924574571E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="F36" s="5"/>
+      <c r="I36" s="10"/>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="F37" s="5"/>
+      <c r="I37" s="10"/>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="F38" s="4"/>
+      <c r="I38" s="10"/>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="F39" s="4"/>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="F40" s="4"/>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="F41" s="4"/>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="F42" s="4"/>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="F43" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>